<commit_message>
Removed forced page breaks for jury
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/jury/Jury-A4.xlsx
+++ b/owlcms/src/main/resources/templates/jury/Jury-A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\jury\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569AC3FC-FEA6-4207-ABF4-AAD2C19A72A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C49C247-EBD9-40FC-BA69-EBE2BEDFF35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jury" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="CategoryFilter">Jury!#REF!</definedName>
     <definedName name="CLUB">Jury!#REF!</definedName>
     <definedName name="Collet">#REF!</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="0">Jury!$A$1:$BY$103</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">Jury!$A$1:$BY$76</definedName>
     <definedName name="demandé">Jury!#REF!</definedName>
     <definedName name="dernier">Jury!#REF!</definedName>
     <definedName name="essais">Jury!#REF!</definedName>
@@ -37,9 +37,9 @@
     <definedName name="InactiveGroupFilter">Jury!#REF!</definedName>
     <definedName name="isSnatch">Jury!#REF!</definedName>
     <definedName name="lbParKg">Jury!#REF!</definedName>
-    <definedName name="LignesCalculs">Jury!$22:$42</definedName>
+    <definedName name="LignesCalculs">Jury!$13:$15</definedName>
     <definedName name="LignesEntête">Jury!$1:$5</definedName>
-    <definedName name="LignesOfficiels">Jury!$12:$20</definedName>
+    <definedName name="LignesOfficiels">Jury!$12:$12</definedName>
     <definedName name="M_F">Jury!#REF!</definedName>
     <definedName name="NAIS.">Jury!#REF!</definedName>
     <definedName name="NbCollet">#REF!</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -150,87 +150,6 @@
   </si>
   <si>
     <t>${t.get("Jury.Signature")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.Score")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.A")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.B")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.C")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.D")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.E")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.F")}</t>
-  </si>
-  <si>
-    <t>Page 1 of 2</t>
-  </si>
-  <si>
-    <t>Page 2 of 2</t>
-  </si>
-  <si>
-    <t>1. ${t.get("Jury.incorrect.1")}</t>
-  </si>
-  <si>
-    <t>2. ${t.get("Jury.incorrect.2")}</t>
-  </si>
-  <si>
-    <t>3. ${t.get("Jury.incorrect.3")}</t>
-  </si>
-  <si>
-    <t>4. ${t.get("Jury.incorrect.4")}</t>
-  </si>
-  <si>
-    <t>5. ${t.get("Jury.incorrect.5")}</t>
-  </si>
-  <si>
-    <t>6. ${t.get("Jury.incorrect.6")}</t>
-  </si>
-  <si>
-    <t>7. ${t.get("Jury.incorrect.7")}</t>
-  </si>
-  <si>
-    <t>8. ${t.get("Jury.incorrect.8")}</t>
-  </si>
-  <si>
-    <t>9. ${t.get("Jury.incorrect.9")}</t>
-  </si>
-  <si>
-    <t>10. ${t.get("Jury.incorrect.10")}</t>
-  </si>
-  <si>
-    <t>11. ${t.get("Jury.incorrect.11")}</t>
-  </si>
-  <si>
-    <t>12. ${t.get("Jury.incorrect.12")}</t>
-  </si>
-  <si>
-    <t>13. ${t.get("Jury.incorrect.13")}</t>
-  </si>
-  <si>
-    <t>14. ${t.get("Jury.incorrect.14")}</t>
-  </si>
-  <si>
-    <t>15. ${t.get("Jury.incorrect.15")}</t>
-  </si>
-  <si>
-    <t>16. ${t.get("Jury.incorrect.16")}</t>
-  </si>
-  <si>
-    <t>17. ${t.get("Jury.incorrect.17")}</t>
-  </si>
-  <si>
-    <t>${t.get("Jury.incorrect.Title")}</t>
   </si>
 </sst>
 </file>
@@ -241,7 +160,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="0;\(0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -318,13 +237,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -352,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -406,34 +318,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="8"/>
       </left>
       <right/>
@@ -481,43 +365,6 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,7 +423,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -641,10 +488,6 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -658,50 +501,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -713,9 +539,28 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -724,38 +569,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -763,26 +577,13 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -920,7 +721,7 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="206464" cy="313295"/>
@@ -1325,10 +1126,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:F33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1347,87 +1148,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="27"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="26"/>
+      <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="26"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="26"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1435,25 +1236,25 @@
       <c r="B6" s="4"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="56" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="56"/>
-      <c r="K6" s="58"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="60"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1466,10 +1267,10 @@
       <c r="G7" s="9">
         <v>2</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="34">
         <v>3</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="31">
         <v>1</v>
       </c>
       <c r="J7" s="9">
@@ -1485,23 +1286,23 @@
       </c>
     </row>
     <row r="9" spans="1:12" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="35" t="s">
+      <c r="C9" s="51"/>
+      <c r="D9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="38"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
@@ -1522,10 +1323,10 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="50"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
       <c r="E12" s="18"/>
@@ -1536,525 +1337,179 @@
       <c r="H12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="26"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="13"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="K14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" s="26"/>
-    </row>
-    <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="26"/>
-    </row>
-    <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-    </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="43"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="26"/>
-    </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-    </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-    </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-    </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-    </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-    </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-    </row>
-    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-    </row>
-    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-    </row>
-    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
-    </row>
-    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-    </row>
-    <row r="37" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="64"/>
-    </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="K38" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+    </row>
+    <row r="20" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+    </row>
+    <row r="21" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+    </row>
+    <row r="22" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+    </row>
+    <row r="23" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+    </row>
+    <row r="24" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="5"/>
     </row>
-    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="5"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
-    </row>
-    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="5"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-    </row>
-    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="5"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-    </row>
-    <row r="49" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C49" s="5"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-    </row>
-    <row r="50" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" s="5"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-    </row>
-    <row r="51" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" s="5"/>
     </row>
-    <row r="60" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="5"/>
     </row>
-    <row r="63" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C63" s="5"/>
     </row>
-    <row r="64" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" s="5"/>
     </row>
     <row r="65" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2099,112 +1554,9 @@
     <row r="78" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" s="5"/>
     </row>
-    <row r="79" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C89" s="5"/>
-    </row>
-    <row r="90" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C92" s="5"/>
-    </row>
-    <row r="93" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C93" s="5"/>
-    </row>
-    <row r="94" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C94" s="5"/>
-    </row>
-    <row r="95" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C95" s="5"/>
-    </row>
-    <row r="96" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C96" s="5"/>
-    </row>
-    <row r="97" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C97" s="5"/>
-    </row>
-    <row r="98" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C98" s="5"/>
-    </row>
-    <row r="99" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C99" s="5"/>
-    </row>
-    <row r="100" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C100" s="5"/>
-    </row>
-    <row r="101" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C101" s="5"/>
-    </row>
-    <row r="102" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C102" s="5"/>
-    </row>
-    <row r="103" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C103" s="5"/>
-    </row>
-    <row r="104" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C104" s="5"/>
-    </row>
-    <row r="105" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C105" s="5"/>
-    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="40">
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="G36:K36"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="G30:K30"/>
+  <mergeCells count="10">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="C4:E4"/>
@@ -2215,32 +1567,24 @@
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:B10">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11 J12:J13 C12:C14 B20:C24 J25 C25:C26 B26:C26 C38">
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
+  <conditionalFormatting sqref="B11:C11 C12 J12">
+    <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D10">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E10">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2254,7 +1598,7 @@
       <formula2>200</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.06" bottom="0.1" header="0" footer="0"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.13" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="83" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>

</xml_diff>